<commit_message>
Code for Version 0.3.0 which adds initial support for JRuby.
</commit_message>
<xml_diff>
--- a/sample_data/Sample Ingest Data.xlsx
+++ b/sample_data/Sample Ingest Data.xlsx
@@ -2020,12 +2020,12 @@
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
+      <alignment vertical="bottom" horizontal="left" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="49" borderId="0" applyFont="1" fontId="1" applyNumberFormat="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
-      <alignment vertical="bottom" horizontal="left" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="49" borderId="0" applyFont="1" fontId="1" applyNumberFormat="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
@@ -6395,7 +6395,7 @@
       <c t="s" s="10" r="H1">
         <v>310</v>
       </c>
-      <c t="s" s="3" r="I1">
+      <c t="s" s="2" r="I1">
         <v>167</v>
       </c>
       <c t="s" s="10" r="J1">
@@ -6436,7 +6436,7 @@
       <c s="4" r="F2">
         <v>2001</v>
       </c>
-      <c t="s" s="1" r="G2">
+      <c t="s" s="3" r="G2">
         <v>315</v>
       </c>
       <c t="s" r="H2">
@@ -6467,7 +6467,7 @@
       </c>
       <c s="4" r="E3"/>
       <c s="4" r="F3"/>
-      <c t="s" s="1" r="G3">
+      <c t="s" s="3" r="G3">
         <v>315</v>
       </c>
       <c t="s" r="H3">
@@ -6490,7 +6490,7 @@
       </c>
       <c s="4" r="E4"/>
       <c s="4" r="F4"/>
-      <c t="s" s="1" r="G4">
+      <c t="s" s="3" r="G4">
         <v>315</v>
       </c>
       <c t="s" r="H4">
@@ -6513,7 +6513,7 @@
       </c>
       <c s="4" r="E5"/>
       <c s="4" r="F5"/>
-      <c t="s" s="1" r="G5">
+      <c t="s" s="3" r="G5">
         <v>315</v>
       </c>
       <c t="s" r="H5">
@@ -6536,7 +6536,7 @@
       </c>
       <c s="4" r="E6"/>
       <c s="4" r="F6"/>
-      <c t="s" s="1" r="G6">
+      <c t="s" s="3" r="G6">
         <v>315</v>
       </c>
       <c t="s" r="H6">
@@ -6559,7 +6559,7 @@
       </c>
       <c s="4" r="E7"/>
       <c s="4" r="F7"/>
-      <c t="s" s="1" r="G7">
+      <c t="s" s="3" r="G7">
         <v>315</v>
       </c>
       <c t="s" r="H7">
@@ -6595,7 +6595,7 @@
       <c s="4" r="F9">
         <v>2002</v>
       </c>
-      <c t="s" s="1" r="G9">
+      <c t="s" s="3" r="G9">
         <v>315</v>
       </c>
       <c t="s" r="H9">
@@ -6627,7 +6627,7 @@
       <c s="4" r="F10">
         <v>2003</v>
       </c>
-      <c t="s" s="1" r="G10">
+      <c t="s" s="3" r="G10">
         <v>315</v>
       </c>
       <c t="s" r="H10">
@@ -6659,7 +6659,7 @@
       <c s="4" r="F11">
         <v>2000</v>
       </c>
-      <c t="s" s="1" r="G11">
+      <c t="s" s="3" r="G11">
         <v>315</v>
       </c>
       <c t="s" r="H11">
@@ -6691,7 +6691,7 @@
       <c s="4" r="F12">
         <v>2001</v>
       </c>
-      <c t="s" s="1" r="G12">
+      <c t="s" s="3" r="G12">
         <v>315</v>
       </c>
       <c t="s" r="H12">
@@ -6723,7 +6723,7 @@
       <c s="4" r="F13">
         <v>2002</v>
       </c>
-      <c t="s" s="1" r="G13">
+      <c t="s" s="3" r="G13">
         <v>315</v>
       </c>
       <c t="s" r="H13">
@@ -6755,7 +6755,7 @@
       <c s="4" r="F14">
         <v>2003</v>
       </c>
-      <c t="s" s="1" r="G14">
+      <c t="s" s="3" r="G14">
         <v>315</v>
       </c>
       <c t="s" r="H14">
@@ -6787,7 +6787,7 @@
       <c s="4" r="F15">
         <v>2004</v>
       </c>
-      <c t="s" s="1" r="G15">
+      <c t="s" s="3" r="G15">
         <v>315</v>
       </c>
       <c t="s" r="H15">
@@ -6819,7 +6819,7 @@
       <c s="4" r="F16">
         <v>2005</v>
       </c>
-      <c t="s" s="1" r="G16">
+      <c t="s" s="3" r="G16">
         <v>315</v>
       </c>
       <c t="s" r="H16">
@@ -6851,7 +6851,7 @@
       <c s="4" r="F17">
         <v>2006</v>
       </c>
-      <c t="s" s="1" r="G17">
+      <c t="s" s="3" r="G17">
         <v>315</v>
       </c>
       <c t="s" r="H17">
@@ -6883,7 +6883,7 @@
       <c s="4" r="F18">
         <v>2007</v>
       </c>
-      <c t="s" s="1" r="G18">
+      <c t="s" s="3" r="G18">
         <v>315</v>
       </c>
       <c t="s" r="H18">
@@ -6915,7 +6915,7 @@
       <c s="4" r="F19">
         <v>2008</v>
       </c>
-      <c t="s" s="1" r="G19">
+      <c t="s" s="3" r="G19">
         <v>315</v>
       </c>
       <c t="s" r="H19">
@@ -6947,7 +6947,7 @@
       <c s="4" r="F20">
         <v>2009</v>
       </c>
-      <c t="s" s="1" r="G20">
+      <c t="s" s="3" r="G20">
         <v>315</v>
       </c>
       <c t="s" r="H20">
@@ -6969,15 +6969,15 @@
     </row>
     <row r="22">
       <c s="4" r="A22"/>
-      <c t="s" s="2" r="B22">
+      <c t="s" s="1" r="B22">
         <v>357</v>
       </c>
-      <c s="2" r="C22"/>
-      <c s="2" r="D22"/>
-      <c s="2" r="E22"/>
-      <c s="2" r="F22"/>
-      <c s="2" r="G22"/>
-      <c s="2" r="H22"/>
+      <c s="1" r="C22"/>
+      <c s="1" r="D22"/>
+      <c s="1" r="E22"/>
+      <c s="1" r="F22"/>
+      <c s="1" r="G22"/>
+      <c s="1" r="H22"/>
       <c s="6" r="I22"/>
     </row>
     <row r="23">
@@ -7006,7 +7006,7 @@
       <c s="4" r="F24">
         <v>2012</v>
       </c>
-      <c t="s" s="1" r="G24">
+      <c t="s" s="3" r="G24">
         <v>315</v>
       </c>
       <c t="s" r="H24">
@@ -7034,7 +7034,7 @@
       </c>
       <c s="4" r="E25"/>
       <c s="4" r="F25"/>
-      <c t="s" s="1" r="G25">
+      <c t="s" s="3" r="G25">
         <v>315</v>
       </c>
       <c t="s" r="H25">
@@ -7059,7 +7059,7 @@
       </c>
       <c s="4" r="E26"/>
       <c s="4" r="F26"/>
-      <c t="s" s="1" r="G26">
+      <c t="s" s="3" r="G26">
         <v>315</v>
       </c>
       <c t="s" r="H26">
@@ -7084,7 +7084,7 @@
       </c>
       <c s="4" r="E27"/>
       <c s="4" r="F27"/>
-      <c t="s" s="1" r="G27">
+      <c t="s" s="3" r="G27">
         <v>315</v>
       </c>
       <c t="s" r="H27">
@@ -7109,7 +7109,7 @@
       </c>
       <c s="4" r="E28"/>
       <c s="4" r="F28"/>
-      <c t="s" s="1" r="G28">
+      <c t="s" s="3" r="G28">
         <v>315</v>
       </c>
       <c t="s" r="H28">
@@ -7134,7 +7134,7 @@
       </c>
       <c s="4" r="E29"/>
       <c s="4" r="F29"/>
-      <c t="s" s="1" r="G29">
+      <c t="s" s="3" r="G29">
         <v>315</v>
       </c>
       <c t="s" r="H29">
@@ -7721,7 +7721,7 @@
       <c t="s" s="9" r="I1">
         <v>376</v>
       </c>
-      <c t="s" s="3" r="J1">
+      <c t="s" s="2" r="J1">
         <v>167</v>
       </c>
       <c t="s" s="10" r="K1">
@@ -7733,7 +7733,7 @@
       <c t="s" s="10" r="M1">
         <v>378</v>
       </c>
-      <c t="s" s="3" r="N1">
+      <c t="s" s="2" r="N1">
         <v>379</v>
       </c>
       <c t="s" s="10" r="O1">
@@ -8383,12 +8383,12 @@
     </row>
     <row r="26">
       <c s="4" r="A26"/>
-      <c t="s" s="2" r="B26">
+      <c t="s" s="1" r="B26">
         <v>450</v>
       </c>
-      <c s="2" r="C26"/>
-      <c s="2" r="D26"/>
-      <c s="2" r="E26"/>
+      <c s="1" r="C26"/>
+      <c s="1" r="D26"/>
+      <c s="1" r="E26"/>
       <c s="4" r="G26"/>
       <c s="4" r="I26"/>
       <c s="6" r="J26"/>
@@ -9553,7 +9553,7 @@
       <c t="s" s="9" r="I1">
         <v>376</v>
       </c>
-      <c t="s" s="3" r="J1">
+      <c t="s" s="2" r="J1">
         <v>167</v>
       </c>
       <c t="s" s="10" r="K1">
@@ -9565,7 +9565,7 @@
       <c t="s" s="10" r="M1">
         <v>524</v>
       </c>
-      <c t="s" s="3" r="N1">
+      <c t="s" s="2" r="N1">
         <v>379</v>
       </c>
       <c t="s" s="10" r="O1">
@@ -10218,9 +10218,9 @@
       <c t="s" s="8" r="B26">
         <v>450</v>
       </c>
-      <c s="2" r="C26"/>
-      <c s="2" r="D26"/>
-      <c s="2" r="E26"/>
+      <c s="1" r="C26"/>
+      <c s="1" r="D26"/>
+      <c s="1" r="E26"/>
       <c s="4" r="G26"/>
       <c s="4" r="I26"/>
       <c s="6" r="J26"/>

</xml_diff>